<commit_message>
Added word information to results; fixed a bug with admin privileges
</commit_message>
<xml_diff>
--- a/groups_exp.xlsx
+++ b/groups_exp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02dd81782c253827/Documents/Dropbox/Project Zhodiac/Goat (production)/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{D2BA77B5-70DB-4E04-AC43-B8443DC6F2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7A4D544F-DBA4-4289-BB31-B7D8CD640268}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{D2BA77B5-70DB-4E04-AC43-B8443DC6F2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B971B4E5-68F8-47C5-8CD7-E84914EC023D}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="2070" windowWidth="14025" windowHeight="11835" xr2:uid="{7D55A6F8-CE01-4330-BBF1-680142604569}"/>
+    <workbookView xWindow="11100" yWindow="2175" windowWidth="14025" windowHeight="11835" activeTab="3" xr2:uid="{7D55A6F8-CE01-4330-BBF1-680142604569}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="2" r:id="rId1"/>
@@ -197,9 +197,6 @@
     <t>That's the shopkeeper that the farmer is really envied by.</t>
   </si>
   <si>
-    <t>That's the shopkeepr that the farmer is really interested by.</t>
-  </si>
-  <si>
     <t>That's the daughter that the father particularly cherishes.</t>
   </si>
   <si>
@@ -471,6 +468,9 @@
   </si>
   <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t>That's the shopkeeper that the farmer is really interested by.</t>
   </si>
 </sst>
 </file>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535432DF-0BDB-45D0-B5E6-FF26C8A6825D}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,33 +852,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -963,7 +963,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -1094,12 +1094,12 @@
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -1111,12 +1111,12 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -1128,12 +1128,12 @@
         <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
@@ -1145,12 +1145,12 @@
         <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
@@ -1162,12 +1162,12 @@
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
@@ -1179,12 +1179,12 @@
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
@@ -1196,12 +1196,12 @@
         <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
@@ -1213,12 +1213,12 @@
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
@@ -1230,12 +1230,12 @@
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" s="1">
         <v>22</v>
@@ -1247,12 +1247,12 @@
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B24" s="1">
         <v>23</v>
@@ -1264,12 +1264,12 @@
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="1">
         <v>24</v>
@@ -1281,12 +1281,12 @@
         <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
@@ -1298,12 +1298,12 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B27" s="1">
         <v>26</v>
@@ -1315,12 +1315,12 @@
         <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B28" s="1">
         <v>27</v>
@@ -1332,12 +1332,12 @@
         <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" s="1">
         <v>28</v>
@@ -1349,12 +1349,12 @@
         <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B30" s="1">
         <v>29</v>
@@ -1366,12 +1366,12 @@
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="1">
         <v>30</v>
@@ -1383,12 +1383,12 @@
         <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B32" s="1">
         <v>31</v>
@@ -1400,12 +1400,12 @@
         <v>5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" s="1">
         <v>32</v>
@@ -1417,7 +1417,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1451,33 +1451,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -1562,7 +1562,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -1693,12 +1693,12 @@
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -1710,12 +1710,12 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -1727,12 +1727,12 @@
         <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
@@ -1744,12 +1744,12 @@
         <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
@@ -1761,12 +1761,12 @@
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
@@ -1778,12 +1778,12 @@
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
@@ -1795,12 +1795,12 @@
         <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
@@ -1812,12 +1812,12 @@
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
@@ -1829,12 +1829,12 @@
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B23" s="1">
         <v>22</v>
@@ -1846,12 +1846,12 @@
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" s="1">
         <v>23</v>
@@ -1863,12 +1863,12 @@
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B25" s="1">
         <v>24</v>
@@ -1880,12 +1880,12 @@
         <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
@@ -1897,12 +1897,12 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" s="1">
         <v>26</v>
@@ -1914,12 +1914,12 @@
         <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="1">
         <v>27</v>
@@ -1931,12 +1931,12 @@
         <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B29" s="1">
         <v>28</v>
@@ -1948,12 +1948,12 @@
         <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B30" s="1">
         <v>29</v>
@@ -1965,12 +1965,12 @@
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B31" s="1">
         <v>30</v>
@@ -1982,12 +1982,12 @@
         <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" s="1">
         <v>31</v>
@@ -1999,12 +1999,12 @@
         <v>5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B33" s="1">
         <v>32</v>
@@ -2016,7 +2016,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2029,7 +2029,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I33"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,33 +2050,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -2178,7 +2178,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -2275,12 +2275,12 @@
         <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -2292,12 +2292,12 @@
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -2309,12 +2309,12 @@
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -2326,12 +2326,12 @@
         <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
@@ -2343,12 +2343,12 @@
         <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
@@ -2360,12 +2360,12 @@
         <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
@@ -2377,12 +2377,12 @@
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
@@ -2394,12 +2394,12 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
@@ -2411,12 +2411,12 @@
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
@@ -2428,12 +2428,12 @@
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" s="1">
         <v>22</v>
@@ -2445,12 +2445,12 @@
         <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" s="1">
         <v>23</v>
@@ -2462,12 +2462,12 @@
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B25" s="1">
         <v>24</v>
@@ -2479,12 +2479,12 @@
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
@@ -2496,12 +2496,12 @@
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" s="1">
         <v>26</v>
@@ -2513,12 +2513,12 @@
         <v>3</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B28" s="1">
         <v>27</v>
@@ -2530,12 +2530,12 @@
         <v>3</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" s="1">
         <v>28</v>
@@ -2547,12 +2547,12 @@
         <v>5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" s="1">
         <v>29</v>
@@ -2564,12 +2564,12 @@
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B31" s="1">
         <v>30</v>
@@ -2581,12 +2581,12 @@
         <v>3</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B32" s="1">
         <v>31</v>
@@ -2598,12 +2598,12 @@
         <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" s="1">
         <v>32</v>
@@ -2615,7 +2615,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2627,8 +2627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B068BFA-13FB-45D7-B19F-50F6C7A104AC}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2649,33 +2649,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -2692,7 +2692,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -2709,7 +2709,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -2760,7 +2760,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -2845,7 +2845,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -2879,7 +2879,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -2891,12 +2891,12 @@
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -2908,12 +2908,12 @@
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -2925,12 +2925,12 @@
         <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
@@ -2942,12 +2942,12 @@
         <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
@@ -2959,12 +2959,12 @@
         <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
@@ -2976,12 +2976,12 @@
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
@@ -2993,12 +2993,12 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
@@ -3010,12 +3010,12 @@
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
@@ -3027,12 +3027,12 @@
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B23" s="1">
         <v>22</v>
@@ -3044,12 +3044,12 @@
         <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" s="1">
         <v>23</v>
@@ -3061,12 +3061,12 @@
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" s="1">
         <v>24</v>
@@ -3078,12 +3078,12 @@
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
@@ -3095,12 +3095,12 @@
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" s="1">
         <v>26</v>
@@ -3112,12 +3112,12 @@
         <v>3</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B28" s="1">
         <v>27</v>
@@ -3129,12 +3129,12 @@
         <v>3</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B29" s="1">
         <v>28</v>
@@ -3146,12 +3146,12 @@
         <v>5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B30" s="1">
         <v>29</v>
@@ -3163,12 +3163,12 @@
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B31" s="1">
         <v>30</v>
@@ -3180,12 +3180,12 @@
         <v>3</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B32" s="1">
         <v>31</v>
@@ -3197,12 +3197,12 @@
         <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" s="1">
         <v>32</v>
@@ -3214,7 +3214,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>